<commit_message>
Changement horaire + mermaid Création de ecole3.slq
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="h:\Users\Simon\Desktop\BD1\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User-Stousignant\Bureau\GitOrganisation\TousignantSimon-BD1\TousignantSimon-BD1.github.io\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF4F44-233F-4B1C-ABC6-48835639273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A309C0EB-213B-4252-8AE9-C08BD00CFB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6EAA84D-6E98-BB4B-8698-E4F48E48897D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6EAA84D-6E98-BB4B-8698-E4F48E48897D}"/>
   </bookViews>
   <sheets>
     <sheet name="horaire" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
   <si>
     <t xml:space="preserve"> Cours </t>
   </si>
@@ -92,9 +92,6 @@
     <t xml:space="preserve"> Requête CRUD </t>
   </si>
   <si>
-    <t xml:space="preserve"> Atelier 3 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Atelier 4 - formatif formel </t>
   </si>
   <si>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Opérations arithmétiques, chaînes, REGEX </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Atelier 3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Atelier 3b</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmmm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,15 +261,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2A1FD46B-E955-4634-A0A1-7A66872FABA8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -594,23 +607,22 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C3:C31"/>
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.375" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="6" max="6" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.3984375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -627,14 +639,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -651,16 +663,16 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
@@ -676,14 +688,14 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -702,14 +714,14 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -725,14 +737,14 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -751,14 +763,14 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -769,19 +781,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -795,19 +807,19 @@
         <v>2.4</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>8</v>
       </c>
@@ -818,19 +830,19 @@
         <v>2.5</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -844,19 +856,19 @@
         <v>2.5</v>
       </c>
       <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
@@ -867,19 +879,19 @@
         <v>2.6</v>
       </c>
       <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -893,19 +905,19 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>12</v>
       </c>
@@ -916,19 +928,19 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -942,19 +954,19 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>14</v>
       </c>
@@ -962,22 +974,22 @@
         <v>45728</v>
       </c>
       <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -991,19 +1003,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>16</v>
       </c>
@@ -1014,19 +1026,19 @@
         <v>4.2</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1040,19 +1052,19 @@
         <v>4.3</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1063,19 +1075,19 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1086,22 +1098,20 @@
         <v>45747</v>
       </c>
       <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
         <v>39</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>40</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1112,19 +1122,19 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1138,19 +1148,19 @@
         <v>5.2</v>
       </c>
       <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1161,19 +1171,19 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
-      <c r="G23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1187,19 +1197,19 @@
         <v>5.3</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
-      <c r="G24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>24</v>
       </c>
@@ -1210,19 +1220,19 @@
         <v>5.3</v>
       </c>
       <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1236,19 +1246,19 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
       </c>
-      <c r="G26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>26</v>
       </c>
@@ -1259,19 +1269,17 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
         <v>9</v>
       </c>
-      <c r="G27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1285,19 +1293,19 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>28</v>
       </c>
@@ -1308,19 +1316,19 @@
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
         <v>9</v>
       </c>
-      <c r="G29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1334,19 +1342,19 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
       </c>
-      <c r="G30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>30</v>
       </c>
@@ -1357,15 +1365,15 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
       </c>
-      <c r="G31" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="G31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>